<commit_message>
deleted some files and updated some changes
</commit_message>
<xml_diff>
--- a/utilis/LoanDetails_Locked.xlsx
+++ b/utilis/LoanDetails_Locked.xlsx
@@ -22,34 +22,37 @@
     <t>Fixed</t>
   </si>
   <si>
-    <t>376000</t>
-  </si>
-  <si>
-    <t>Attached</t>
-  </si>
-  <si>
-    <t>LP</t>
-  </si>
-  <si>
-    <t>F_DEEPIKA_23SEP_25_006</t>
-  </si>
-  <si>
-    <t>L_DEEPIKA_23SEP_25_006</t>
+    <t>180000</t>
+  </si>
+  <si>
+    <t>Detached</t>
+  </si>
+  <si>
+    <t>DU</t>
+  </si>
+  <si>
+    <t>Denis</t>
+  </si>
+  <si>
+    <t>TPO_Y</t>
   </si>
   <si>
     <t>Null Value</t>
   </si>
   <si>
-    <t>96.50</t>
-  </si>
-  <si>
-    <t>Chicago</t>
-  </si>
-  <si>
-    <t>46.812</t>
-  </si>
-  <si>
-    <t>800</t>
+    <t>94.31</t>
+  </si>
+  <si>
+    <t>Blue Island</t>
+  </si>
+  <si>
+    <t>10.0</t>
+  </si>
+  <si>
+    <t>777</t>
+  </si>
+  <si>
+    <t>true</t>
   </si>
   <si>
     <t>false</t>
@@ -58,10 +61,10 @@
     <t>TI</t>
   </si>
   <si>
-    <t>362840</t>
-  </si>
-  <si>
-    <t>TestSigma_29-09-2025_SC1_23_544</t>
+    <t>169750</t>
+  </si>
+  <si>
+    <t>DEN_20251006_10001_TPO_Y</t>
   </si>
   <si>
     <t>Purchase</t>
@@ -70,52 +73,52 @@
     <t>360</t>
   </si>
   <si>
-    <t>5445.42</t>
-  </si>
-  <si>
-    <t>FHA</t>
-  </si>
-  <si>
-    <t>6.875</t>
-  </si>
-  <si>
-    <t>4</t>
+    <t>Conventional</t>
+  </si>
+  <si>
+    <t>7.500</t>
+  </si>
+  <si>
+    <t>1</t>
   </si>
   <si>
     <t>PrimaryResidence</t>
   </si>
   <si>
-    <t>110_20/25/30 Yr FHA Fixed-GNMA II</t>
-  </si>
-  <si>
-    <t>UnitDwelling_2_4</t>
+    <t>212_25/30 Yr Fannie Mae Fixed</t>
+  </si>
+  <si>
+    <t>SingleFamily</t>
+  </si>
+  <si>
+    <t>175000</t>
   </si>
   <si>
     <t>IL</t>
   </si>
   <si>
-    <t>4248 W Wilcox St</t>
+    <t>12714 Mozart St</t>
   </si>
   <si>
     <t>0</t>
   </si>
   <si>
-    <t>60624</t>
-  </si>
-  <si>
-    <t>110</t>
+    <t>60406</t>
+  </si>
+  <si>
+    <t>212</t>
   </si>
   <si>
     <t>A4187</t>
   </si>
   <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>[3]</t>
-  </si>
-  <si>
-    <t>2606.00</t>
+    <t>15</t>
+  </si>
+  <si>
+    <t>[15]</t>
+  </si>
+  <si>
+    <t>8234.00</t>
   </si>
   <si>
     <t>16984</t>
@@ -133,13 +136,10 @@
     <t>COOK</t>
   </si>
   <si>
-    <t>true</t>
-  </si>
-  <si>
-    <t>BT</t>
-  </si>
-  <si>
-    <t>1.24022</t>
+    <t>T</t>
+  </si>
+  <si>
+    <t>1.3</t>
   </si>
   <si>
     <t>-0.04</t>
@@ -631,7 +631,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -639,7 +639,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -663,7 +663,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -671,7 +671,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -679,7 +679,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -687,7 +687,7 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -695,7 +695,7 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -759,7 +759,7 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>3</v>
+        <v>26</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
@@ -767,7 +767,7 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
@@ -775,7 +775,7 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
@@ -783,7 +783,7 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
@@ -799,7 +799,7 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
@@ -807,7 +807,7 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
@@ -815,7 +815,7 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
@@ -823,7 +823,7 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
@@ -831,7 +831,7 @@
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
@@ -839,7 +839,7 @@
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
@@ -847,7 +847,7 @@
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
@@ -855,7 +855,7 @@
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
@@ -863,7 +863,7 @@
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
@@ -871,7 +871,7 @@
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
@@ -879,7 +879,7 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
@@ -887,7 +887,7 @@
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
@@ -895,7 +895,7 @@
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
@@ -903,7 +903,7 @@
         <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>40</v>
+        <v>13</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
@@ -927,7 +927,7 @@
         <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>40</v>
+        <v>13</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>